<commit_message>
fixed data, preset summary page
</commit_message>
<xml_diff>
--- a/ghg_data.xlsx
+++ b/ghg_data.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27823"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://scotsconnect.sharepoint.com/sites/AgriculturalAnalysisUnit-SG/Shared Documents/Economic Statistics/Data lab 2024/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="27" documentId="13_ncr:1_{86E1618C-7621-4AB3-BEB8-F4A45C08B02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BF84D28C-9203-44BD-B34B-6FF7F4DB0534}"/>
+  <xr:revisionPtr revIDLastSave="46" documentId="13_ncr:1_{86E1618C-7621-4AB3-BEB8-F4A45C08B02D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0F35EFCA-8F05-436D-9F8A-714A2216AFDE}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="subsector_total" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="53">
+  <si>
+    <t>Subsector</t>
+  </si>
   <si>
     <t>1990</t>
   </si>
@@ -167,6 +170,12 @@
     <t>Liming</t>
   </si>
   <si>
+    <t>Urea application</t>
+  </si>
+  <si>
+    <t>Non-energy products from fuels and solvent use</t>
+  </si>
+  <si>
     <t>Other emission source</t>
   </si>
   <si>
@@ -189,21 +198,6 @@
   </si>
   <si>
     <t>Waste Management</t>
-  </si>
-  <si>
-    <t>TOTAL</t>
-  </si>
-  <si>
-    <t>Total (RHS)</t>
-  </si>
-  <si>
-    <t>Subsector</t>
-  </si>
-  <si>
-    <t>Urea application</t>
-  </si>
-  <si>
-    <t>Non-energy products from fuels and solvent use</t>
   </si>
 </sst>
 </file>
@@ -211,12 +205,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="4">
-    <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="164" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="0.0000"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_(* #,##0.0_);_(* \(#,##0.0\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="166" formatCode="_-* #,##0.0_-;\-* #,##0.0_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="167" formatCode="0.0000"/>
   </numFmts>
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -720,19 +714,19 @@
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="166" fontId="19" fillId="33" borderId="0" xfId="43" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="167" fontId="19" fillId="33" borderId="0" xfId="43" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="44">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1093,103 +1087,103 @@
   <dimension ref="A1:AB21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+      <selection activeCell="AA9" sqref="AA9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="14.1796875" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28">
       <c r="A1" t="s">
-        <v>52</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" s="1">
         <v>1.3651867476599404</v>
@@ -1273,9 +1267,9 @@
         <v>1.5617356161264462</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B3" s="1">
         <v>1.6008929089111501</v>
@@ -1359,9 +1353,9 @@
         <v>1.3373176983204711</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B4" s="1">
         <v>0.2857570221328512</v>
@@ -1445,9 +1439,9 @@
         <v>0.23615927032838305</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B5" s="1">
         <v>0.28532248147229827</v>
@@ -1531,9 +1525,9 @@
         <v>0.24965326393502763</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:28">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B6" s="1">
         <v>1.4398832065843781</v>
@@ -1617,9 +1611,9 @@
         <v>1.1901574816942444</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:28">
       <c r="A7" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B7" s="1">
         <v>3.79651216493939</v>
@@ -1703,9 +1697,9 @@
         <v>3.1567829094319477</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:28">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B8" s="1">
         <v>8.7735545317000074</v>
@@ -1789,7 +1783,7 @@
         <v>7.7316528596353935</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:28">
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
       <c r="G15" s="1"/>
@@ -1797,7 +1791,7 @@
       <c r="J15" s="1"/>
       <c r="K15" s="1"/>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:28">
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
       <c r="G16" s="1"/>
@@ -1805,7 +1799,7 @@
       <c r="J16" s="1"/>
       <c r="K16" s="1"/>
     </row>
-    <row r="17" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="17" spans="5:11">
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1813,7 +1807,7 @@
       <c r="J17" s="1"/>
       <c r="K17" s="1"/>
     </row>
-    <row r="18" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="18" spans="5:11">
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1821,7 +1815,7 @@
       <c r="J18" s="1"/>
       <c r="K18" s="1"/>
     </row>
-    <row r="19" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="19" spans="5:11">
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1829,7 +1823,7 @@
       <c r="J19" s="1"/>
       <c r="K19" s="1"/>
     </row>
-    <row r="20" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="20" spans="5:11">
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
       <c r="G20" s="1"/>
@@ -1837,7 +1831,7 @@
       <c r="J20" s="1"/>
       <c r="K20" s="1"/>
     </row>
-    <row r="21" spans="5:11" x14ac:dyDescent="0.35">
+    <row r="21" spans="5:11">
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
       <c r="G21" s="1"/>
@@ -1858,98 +1852,98 @@
       <selection activeCell="D1" sqref="D1:E1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="17.54296875" customWidth="1"/>
-    <col min="2" max="2" width="18.1796875" customWidth="1"/>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28">
       <c r="B1" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B2">
         <v>5.4180778830535878</v>
@@ -2033,9 +2027,9 @@
         <v>4.566182282074629</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:28">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B3">
         <v>0.92926831219735828</v>
@@ -2119,9 +2113,9 @@
         <v>1.2954437181488745</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:28">
       <c r="A4" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B4">
         <v>2.4274043728701398</v>
@@ -2205,9 +2199,9 @@
         <v>1.8700268594118903</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:28">
       <c r="A5" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>8.7747505681210853</v>
@@ -2300,42 +2294,42 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1D035A32-940D-448C-AFC9-C7903F1F1FD1}">
   <dimension ref="A1:G9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="42.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="42.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7">
       <c r="A1" s="2" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="G1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7">
       <c r="A2" s="4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="B2" s="3">
         <v>2.1076099553035883</v>
@@ -2356,9 +2350,9 @@
         <v>0.15863407789027723</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7">
       <c r="A3" s="4" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3">
         <v>0.52841184778067662</v>
@@ -2379,9 +2373,9 @@
         <v>3.9774450264973463E-2</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7">
       <c r="A4" s="4" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B4" s="3">
         <v>0.35450978689695345</v>
@@ -2402,9 +2396,9 @@
         <v>2.5248086549775988E-2</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7">
       <c r="A5" s="4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B5" s="3">
         <v>0.11954734734543523</v>
@@ -2425,9 +2419,9 @@
         <v>8.9931856628213281E-3</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7">
       <c r="A6" s="4" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B6" s="3">
         <v>4.4426988650566733E-2</v>
@@ -2448,9 +2442,9 @@
         <v>3.3410540245344907E-3</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7">
       <c r="A7" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B7">
         <v>2.2769834547274504E-3</v>
@@ -2471,9 +2465,9 @@
         <v>1.6841593600055107E-4</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7">
       <c r="A8" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="B8">
         <v>0</v>
@@ -2494,9 +2488,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:7">
       <c r="A9" s="4" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3">
         <v>2.2769834547274504E-3</v>
@@ -2524,854 +2518,789 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA0F0614-0830-4CE6-BB89-6D904659A044}">
-  <dimension ref="A1:AB10"/>
+  <dimension ref="A1:AB9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9:XFD9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A10" sqref="A10:XFD10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.45"/>
   <cols>
-    <col min="1" max="1" width="18.81640625" customWidth="1"/>
+    <col min="1" max="1" width="18.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:28" ht="15">
       <c r="A1" s="2" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I1" s="2" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="L1" s="2" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="M1" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="O1" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="P1" s="2" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="R1" s="2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="S1" s="2" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="V1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="W1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="X1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="Y1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="Z1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="AA1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="AB1">
         <v>2022</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:28" ht="15">
       <c r="A2" s="3" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B2" s="5">
-        <v>8.7747505681210853</v>
+        <v>8.7747505681210995</v>
       </c>
       <c r="C2" s="5">
-        <v>8.8244783915151572</v>
+        <v>8.8244783915151999</v>
       </c>
       <c r="D2" s="5">
-        <v>9.0147926666662759</v>
+        <v>9.0147926666663007</v>
       </c>
       <c r="E2" s="5">
-        <v>8.9459392452568807</v>
+        <v>8.9459392452569002</v>
       </c>
       <c r="F2" s="5">
-        <v>8.779950665299479</v>
+        <v>8.7799506652995003</v>
       </c>
       <c r="G2" s="5">
-        <v>8.5558906037893365</v>
+        <v>8.5558906037892992</v>
       </c>
       <c r="H2" s="5">
-        <v>8.5569140842555758</v>
+        <v>8.5569140842556006</v>
       </c>
       <c r="I2" s="5">
-        <v>8.5979922377858493</v>
+        <v>8.5979922377857996</v>
       </c>
       <c r="J2" s="5">
-        <v>8.6736868514798626</v>
+        <v>8.6736868514798999</v>
       </c>
       <c r="K2" s="5">
-        <v>8.7612751680331211</v>
+        <v>8.7612751680330998</v>
       </c>
       <c r="L2" s="5">
-        <v>8.4894495377679782</v>
+        <v>8.4894495377679995</v>
       </c>
       <c r="M2" s="5">
-        <v>8.5683107977366362</v>
+        <v>8.5683107977367001</v>
       </c>
       <c r="N2" s="5">
-        <v>8.4471150396527435</v>
+        <v>8.4471150396527008</v>
       </c>
       <c r="O2" s="5">
-        <v>8.4173861583101868</v>
+        <v>8.4173861583101992</v>
       </c>
       <c r="P2" s="5">
-        <v>8.2797626839517502</v>
+        <v>8.2797626839517005</v>
       </c>
       <c r="Q2" s="5">
-        <v>8.113334242412261</v>
+        <v>8.1133342424072001</v>
       </c>
       <c r="R2" s="5">
-        <v>8.1907639962089345</v>
+        <v>8.1907639962089007</v>
       </c>
       <c r="S2" s="5">
-        <v>7.8879053908367984</v>
+        <v>7.8879053908368002</v>
       </c>
       <c r="T2" s="5">
-        <v>8.1036648164740051</v>
+        <v>8.1036648164739997</v>
       </c>
       <c r="U2" s="5">
-        <v>8.1929718450843545</v>
+        <v>8.1929718450844007</v>
       </c>
       <c r="V2">
-        <v>8.030632166894927</v>
+        <v>8.0306321668949003</v>
       </c>
       <c r="W2">
-        <v>7.9512805016062229</v>
+        <v>7.9512805016061998</v>
       </c>
       <c r="X2">
-        <v>7.8862408844826062</v>
+        <v>7.8862408844826</v>
       </c>
       <c r="Y2">
-        <v>7.8940099361449612</v>
+        <v>7.8940099361450002</v>
       </c>
       <c r="Z2">
-        <v>7.870506597217573</v>
+        <v>7.8705065972175996</v>
       </c>
       <c r="AA2">
-        <v>7.9856748926575731</v>
+        <v>7.9856748926575998</v>
       </c>
       <c r="AB2">
-        <v>7.7316528596353944</v>
-      </c>
-    </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
+        <v>7.7316528596353997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="15">
       <c r="A3" s="3" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="B3" s="5">
-        <v>11.498854667890893</v>
+        <v>11.214586636942499</v>
       </c>
       <c r="C3" s="5">
-        <v>11.480804991034722</v>
+        <v>11.072942223305599</v>
       </c>
       <c r="D3" s="5">
-        <v>11.521592492310578</v>
+        <v>11.2248860581608</v>
       </c>
       <c r="E3" s="5">
-        <v>11.535520770205949</v>
+        <v>11.301000689583301</v>
       </c>
       <c r="F3" s="5">
-        <v>11.265184804542669</v>
+        <v>11.048658802130699</v>
       </c>
       <c r="G3" s="5">
-        <v>11.802722818499994</v>
+        <v>11.631493347422801</v>
       </c>
       <c r="H3" s="5">
-        <v>10.705145926806303</v>
+        <v>10.514820520569099</v>
       </c>
       <c r="I3" s="5">
-        <v>10.657758857823902</v>
+        <v>10.4706750717906</v>
       </c>
       <c r="J3" s="5">
-        <v>10.924366692770583</v>
+        <v>10.739582004938301</v>
       </c>
       <c r="K3" s="5">
-        <v>10.947032773406924</v>
+        <v>10.916845964888999</v>
       </c>
       <c r="L3" s="5">
-        <v>10.506268893411351</v>
+        <v>10.6516482467753</v>
       </c>
       <c r="M3" s="5">
-        <v>10.171235132848611</v>
+        <v>10.4090647927642</v>
       </c>
       <c r="N3" s="5">
-        <v>10.699699975196875</v>
+        <v>10.956079271059799</v>
       </c>
       <c r="O3" s="5">
-        <v>10.057653776839421</v>
+        <v>10.186246830064899</v>
       </c>
       <c r="P3" s="5">
-        <v>11.104868504125662</v>
+        <v>11.3741483377094</v>
       </c>
       <c r="Q3" s="5">
-        <v>9.3286331724094538</v>
+        <v>9.5480357378876999</v>
       </c>
       <c r="R3" s="5">
-        <v>10.1714097694159</v>
+        <v>10.3879491013672</v>
       </c>
       <c r="S3" s="5">
-        <v>10.101285528061389</v>
+        <v>10.447651802018999</v>
       </c>
       <c r="T3" s="5">
-        <v>8.6211312427746911</v>
+        <v>8.8640857370519992</v>
       </c>
       <c r="U3" s="5">
-        <v>8.9348736458097395</v>
+        <v>9.2079013161018004</v>
       </c>
       <c r="V3">
-        <v>9.0986715571380508</v>
+        <v>9.1047961775283994</v>
       </c>
       <c r="W3">
-        <v>8.827630182011788</v>
+        <v>9.0552607321188994</v>
       </c>
       <c r="X3">
-        <v>9.0191823833265321</v>
+        <v>9.1271353094453005</v>
       </c>
       <c r="Y3">
-        <v>8.782917433426185</v>
+        <v>8.9791615896128008</v>
       </c>
       <c r="Z3">
-        <v>8.5110092876941756</v>
+        <v>8.5699092540035</v>
       </c>
       <c r="AA3">
-        <v>9.0271802230472886</v>
-      </c>
-    </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
+        <v>8.8604336886156005</v>
+      </c>
+      <c r="AB3">
+        <v>7.6661457864673004</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="15">
       <c r="A4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B4" s="5">
+        <v>14.742174670704101</v>
+      </c>
+      <c r="C4" s="5">
+        <v>16.7201879617378</v>
+      </c>
+      <c r="D4" s="5">
+        <v>17.796323220295299</v>
+      </c>
+      <c r="E4" s="5">
+        <v>16.705530458819101</v>
+      </c>
+      <c r="F4" s="5">
+        <v>19.641552032325801</v>
+      </c>
+      <c r="G4" s="5">
+        <v>18.8596843071808</v>
+      </c>
+      <c r="H4" s="5">
+        <v>17.2026199546527</v>
+      </c>
+      <c r="I4" s="5">
+        <v>17.601432954283901</v>
+      </c>
+      <c r="J4" s="5">
+        <v>15.781024193331801</v>
+      </c>
+      <c r="K4" s="5">
+        <v>14.0414560336327</v>
+      </c>
+      <c r="L4" s="5">
+        <v>18.7543240208283</v>
+      </c>
+      <c r="M4" s="5">
+        <v>15.5456453533186</v>
+      </c>
+      <c r="N4" s="5">
+        <v>14.2657440277564</v>
+      </c>
+      <c r="O4" s="5">
+        <v>13.363582989290601</v>
+      </c>
+      <c r="P4" s="5">
+        <v>15.7648258757807</v>
+      </c>
+      <c r="Q4" s="5">
+        <v>12.060620842016499</v>
+      </c>
+      <c r="R4" s="5">
+        <v>12.745677801370199</v>
+      </c>
+      <c r="S4" s="5">
+        <v>11.379070342428699</v>
+      </c>
+      <c r="T4" s="5">
+        <v>9.7613744688921003</v>
+      </c>
+      <c r="U4" s="5">
+        <v>7.6852051041714997</v>
+      </c>
+      <c r="V4">
+        <v>2.4449608260942002</v>
+      </c>
+      <c r="W4">
+        <v>1.1019351127388</v>
+      </c>
+      <c r="X4">
+        <v>2.0889152929180002</v>
+      </c>
+      <c r="Y4">
+        <v>1.9749936621274</v>
+      </c>
+      <c r="Z4">
+        <v>1.7236731248346</v>
+      </c>
+      <c r="AA4">
+        <v>1.5794309103324</v>
+      </c>
+      <c r="AB4">
+        <v>1.7497526978711</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="15">
+      <c r="A5" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B4" s="5">
-        <v>14.745196186718507</v>
-      </c>
-      <c r="C4" s="5">
-        <v>16.726691842855139</v>
-      </c>
-      <c r="D4" s="5">
-        <v>17.797891931899901</v>
-      </c>
-      <c r="E4" s="5">
-        <v>16.709756350179084</v>
-      </c>
-      <c r="F4" s="5">
-        <v>19.657637916371307</v>
-      </c>
-      <c r="G4" s="5">
-        <v>18.876693822392735</v>
-      </c>
-      <c r="H4" s="5">
-        <v>17.22126555898053</v>
-      </c>
-      <c r="I4" s="5">
-        <v>17.623612554281696</v>
-      </c>
-      <c r="J4" s="5">
-        <v>15.801477309393508</v>
-      </c>
-      <c r="K4" s="5">
-        <v>14.057353011582435</v>
-      </c>
-      <c r="L4" s="5">
-        <v>18.763655443824685</v>
-      </c>
-      <c r="M4" s="5">
-        <v>15.557569538874201</v>
-      </c>
-      <c r="N4" s="5">
-        <v>14.279241101900697</v>
-      </c>
-      <c r="O4" s="5">
-        <v>13.376615155635504</v>
-      </c>
-      <c r="P4" s="5">
-        <v>15.777770400467881</v>
-      </c>
-      <c r="Q4" s="5">
-        <v>12.07312248367028</v>
-      </c>
-      <c r="R4" s="5">
-        <v>12.752295188421979</v>
-      </c>
-      <c r="S4" s="5">
-        <v>11.386746975917697</v>
-      </c>
-      <c r="T4" s="5">
-        <v>9.7720850104425487</v>
-      </c>
-      <c r="U4" s="5">
-        <v>7.692294527130592</v>
-      </c>
-      <c r="V4">
-        <v>2.451450199236394</v>
-      </c>
-      <c r="W4">
-        <v>1.1088894688363871</v>
-      </c>
-      <c r="X4">
-        <v>2.097270762609905</v>
-      </c>
-      <c r="Y4">
-        <v>2.0049986341397594</v>
-      </c>
-      <c r="Z4">
-        <v>1.7263683559259648</v>
-      </c>
-      <c r="AA4">
-        <v>1.6018635758390429</v>
-      </c>
-    </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A5" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="B5" s="5">
-        <v>19.483954809262521</v>
+        <v>19.310838673436798</v>
       </c>
       <c r="C5" s="5">
-        <v>17.221327402434628</v>
+        <v>17.1340892944487</v>
       </c>
       <c r="D5" s="5">
-        <v>17.147203968097916</v>
+        <v>16.706506735122101</v>
       </c>
       <c r="E5" s="5">
-        <v>16.232961505299741</v>
+        <v>15.650991262200099</v>
       </c>
       <c r="F5" s="5">
-        <v>16.544400619716729</v>
+        <v>15.918623446879201</v>
       </c>
       <c r="G5" s="5">
-        <v>16.611462603359413</v>
+        <v>15.913426171906901</v>
       </c>
       <c r="H5" s="5">
-        <v>15.617491869320876</v>
+        <v>15.002736814236499</v>
       </c>
       <c r="I5" s="5">
-        <v>15.583010953685589</v>
+        <v>14.9668448882038</v>
       </c>
       <c r="J5" s="5">
-        <v>15.546748079999663</v>
+        <v>14.8839312738823</v>
       </c>
       <c r="K5" s="5">
-        <v>16.124550400928726</v>
+        <v>15.4361385341162</v>
       </c>
       <c r="L5" s="5">
-        <v>14.891839476870143</v>
+        <v>14.2343643088343</v>
       </c>
       <c r="M5" s="5">
-        <v>14.346254970083683</v>
+        <v>13.792933603752401</v>
       </c>
       <c r="N5" s="5">
-        <v>13.842375039033021</v>
+        <v>13.282053162148401</v>
       </c>
       <c r="O5" s="5">
-        <v>12.223177130426594</v>
+        <v>11.609704325492</v>
       </c>
       <c r="P5" s="5">
-        <v>12.409070144662067</v>
+        <v>11.8425577298531</v>
       </c>
       <c r="Q5" s="5">
-        <v>11.906374234972336</v>
+        <v>11.357445534832699</v>
       </c>
       <c r="R5" s="5">
-        <v>11.363483689491963</v>
+        <v>10.834163992172099</v>
       </c>
       <c r="S5" s="5">
-        <v>11.358775568842965</v>
+        <v>10.927576086803599</v>
       </c>
       <c r="T5" s="5">
-        <v>10.59146818421643</v>
+        <v>10.117438745134001</v>
       </c>
       <c r="U5" s="5">
-        <v>10.711563123732258</v>
+        <v>10.2598219078479</v>
       </c>
       <c r="V5">
-        <v>11.257968757768163</v>
+        <v>10.666163884203501</v>
       </c>
       <c r="W5">
-        <v>11.480471060284394</v>
+        <v>10.8679844092657</v>
       </c>
       <c r="X5">
-        <v>11.321634745244916</v>
+        <v>10.7821969282704</v>
       </c>
       <c r="Y5">
-        <v>10.584054028726634</v>
+        <v>9.9808033750915008</v>
       </c>
       <c r="Z5">
-        <v>10.2247321942626</v>
+        <v>9.5461361585683999</v>
       </c>
       <c r="AA5">
-        <v>9.6085561055850306</v>
-      </c>
-    </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
+        <v>8.8470840312869008</v>
+      </c>
+      <c r="AB5">
+        <v>8.7906228372787005</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" ht="15">
       <c r="A6" s="3" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="B6" s="5">
-        <v>6.0371137009626583</v>
+        <v>5.9802620215038003</v>
       </c>
       <c r="C6" s="5">
-        <v>4.2158159577336694</v>
+        <v>4.1528466003908999</v>
       </c>
       <c r="D6" s="5">
-        <v>2.9329551461213295</v>
+        <v>2.8653894634936998</v>
       </c>
       <c r="E6" s="5">
-        <v>2.4080060073539946</v>
+        <v>2.3390641294046</v>
       </c>
       <c r="F6" s="5">
-        <v>2.233818478223327</v>
+        <v>2.1685931351817</v>
       </c>
       <c r="G6" s="5">
-        <v>1.8941105776699987</v>
+        <v>1.8289921228073001</v>
       </c>
       <c r="H6" s="5">
-        <v>1.4390405675380111</v>
+        <v>1.3737474618634999</v>
       </c>
       <c r="I6" s="5">
-        <v>1.4467367682583376</v>
+        <v>1.3808595673385</v>
       </c>
       <c r="J6" s="5">
-        <v>1.1011988097990049</v>
+        <v>1.0364202441359001</v>
       </c>
       <c r="K6" s="5">
-        <v>0.88429818712966068</v>
+        <v>0.81995222791940003</v>
       </c>
       <c r="L6" s="5">
-        <v>0.52628977672234223</v>
+        <v>0.46159751779059999</v>
       </c>
       <c r="M6" s="5">
-        <v>0.32314043749799382</v>
+        <v>0.25867849693430001</v>
       </c>
       <c r="N6" s="5">
-        <v>8.7251699956985895E-2</v>
+        <v>2.3496786422599999E-2</v>
       </c>
       <c r="O6" s="5">
-        <v>7.6712786136690081E-3</v>
+        <v>-5.6584505632000001E-2</v>
       </c>
       <c r="P6" s="5">
-        <v>-3.3184778243659396E-2</v>
+        <v>-9.7493198352199995E-2</v>
       </c>
       <c r="Q6" s="5">
-        <v>-0.34055481716866898</v>
+        <v>-0.40593878428180002</v>
       </c>
       <c r="R6" s="5">
-        <v>-0.44925979901232838</v>
+        <v>-0.52426535107100003</v>
       </c>
       <c r="S6" s="5">
-        <v>-7.484318998133288E-2</v>
+        <v>-0.16137774188779999</v>
       </c>
       <c r="T6" s="5">
-        <v>-0.2900886370679967</v>
+        <v>-0.38337144769710002</v>
       </c>
       <c r="U6" s="5">
-        <v>0.22700132493499225</v>
+        <v>0.1153190906326</v>
       </c>
       <c r="V6">
-        <v>-0.11911552324634367</v>
+        <v>-0.22073449547390001</v>
       </c>
       <c r="W6">
-        <v>-0.10599636616566999</v>
+        <v>-0.21031512870630001</v>
       </c>
       <c r="X6">
-        <v>0.43886797175066561</v>
+        <v>0.28202817178840001</v>
       </c>
       <c r="Y6">
-        <v>0.94708995738498936</v>
+        <v>0.85633763433190002</v>
       </c>
       <c r="Z6">
-        <v>0.31881778534933081</v>
+        <v>0.20211950812310001</v>
       </c>
       <c r="AA6">
-        <v>0.35817458245066325</v>
-      </c>
-    </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
+        <v>3.5639831877399997E-2</v>
+      </c>
+      <c r="AB6">
+        <v>0.21865375463549999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" ht="15">
       <c r="A7" s="3" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B7" s="5">
-        <v>14.886066617639221</v>
+        <v>14.8316925025513</v>
       </c>
       <c r="C7" s="5">
-        <v>15.845730231889453</v>
+        <v>15.8044467145626</v>
       </c>
       <c r="D7" s="5">
-        <v>16.492757575698295</v>
+        <v>16.423352748273899</v>
       </c>
       <c r="E7" s="5">
-        <v>16.415391190510473</v>
+        <v>16.3460035713431</v>
       </c>
       <c r="F7" s="5">
-        <v>15.703643990089178</v>
+        <v>15.6402625117121</v>
       </c>
       <c r="G7" s="5">
-        <v>15.529486616039497</v>
+        <v>15.478381541947501</v>
       </c>
       <c r="H7" s="5">
-        <v>15.896873088865142</v>
+        <v>15.8630154998426</v>
       </c>
       <c r="I7" s="5">
-        <v>15.648924108132698</v>
+        <v>15.6145373623373</v>
       </c>
       <c r="J7" s="5">
-        <v>15.603714027114139</v>
+        <v>15.5676328013381</v>
       </c>
       <c r="K7" s="5">
-        <v>15.748129685192019</v>
+        <v>15.714149969825399</v>
       </c>
       <c r="L7" s="5">
-        <v>15.702328235953127</v>
+        <v>15.666413131855</v>
       </c>
       <c r="M7" s="5">
-        <v>15.979610979924248</v>
+        <v>15.9339236795927</v>
       </c>
       <c r="N7" s="5">
-        <v>15.43900983488062</v>
+        <v>15.3985354050475</v>
       </c>
       <c r="O7" s="5">
-        <v>14.762767400893225</v>
+        <v>14.729164937272399</v>
       </c>
       <c r="P7" s="5">
-        <v>14.277991313239689</v>
+        <v>14.2178406801427</v>
       </c>
       <c r="Q7" s="5">
-        <v>13.849548595110511</v>
+        <v>13.7992325781275</v>
       </c>
       <c r="R7" s="5">
-        <v>13.588267980276678</v>
+        <v>13.5162927867098</v>
       </c>
       <c r="S7" s="5">
-        <v>13.444821472516315</v>
+        <v>13.354369474022301</v>
       </c>
       <c r="T7" s="5">
-        <v>13.683866086472026</v>
+        <v>13.6072019956113</v>
       </c>
       <c r="U7" s="5">
-        <v>13.982164946616418</v>
+        <v>13.906121800095301</v>
       </c>
       <c r="V7">
-        <v>14.41679636307609</v>
+        <v>14.327414921443101</v>
       </c>
       <c r="W7">
-        <v>14.738231063111495</v>
+        <v>14.7639846479801</v>
       </c>
       <c r="X7">
-        <v>14.592572826218349</v>
+        <v>14.629309316265401</v>
       </c>
       <c r="Y7">
-        <v>14.430086558553469</v>
+        <v>14.472840908335201</v>
       </c>
       <c r="Z7">
-        <v>10.712953212185869</v>
+        <v>10.730456399283399</v>
       </c>
       <c r="AA7">
-        <v>11.644931999503036</v>
-      </c>
-    </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
+        <v>11.7833186221294</v>
+      </c>
+      <c r="AB7">
+        <v>12.860689303200401</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" ht="15">
       <c r="A8" s="3" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="B8" s="5">
-        <v>6.5009803514860351</v>
+        <v>6.5015883902646001</v>
       </c>
       <c r="C8" s="5">
-        <v>6.7620240064343333</v>
+        <v>6.7627284954407001</v>
       </c>
       <c r="D8" s="5">
-        <v>6.5774531986725169</v>
+        <v>6.5780604692314997</v>
       </c>
       <c r="E8" s="5">
-        <v>6.30112067225883</v>
+        <v>6.3016942545751</v>
       </c>
       <c r="F8" s="5">
-        <v>6.1349141349238048</v>
+        <v>6.1354557719225999</v>
       </c>
       <c r="G8" s="5">
-        <v>5.8203692607283424</v>
+        <v>5.8208495864326997</v>
       </c>
       <c r="H8" s="5">
-        <v>5.6201778853762896</v>
+        <v>5.6206263320516001</v>
       </c>
       <c r="I8" s="5">
-        <v>5.4979868310795021</v>
+        <v>5.4983890218329998</v>
       </c>
       <c r="J8" s="5">
-        <v>4.7757639771393254</v>
+        <v>4.7761523262691998</v>
       </c>
       <c r="K8" s="5">
-        <v>4.3253955504579764</v>
+        <v>4.3257467991108998</v>
       </c>
       <c r="L8" s="5">
-        <v>3.8881260294870899</v>
+        <v>3.8884180643503998</v>
       </c>
       <c r="M8" s="5">
-        <v>3.4922311507230677</v>
+        <v>3.4946911346984</v>
       </c>
       <c r="N8" s="5">
-        <v>3.323601411865678</v>
+        <v>3.3257782129511</v>
       </c>
       <c r="O8" s="5">
-        <v>2.9747127075540729</v>
+        <v>2.9768160187997998</v>
       </c>
       <c r="P8" s="5">
-        <v>2.7185733282709474</v>
+        <v>2.7199287963968</v>
       </c>
       <c r="Q8" s="5">
-        <v>2.5606806276791172</v>
+        <v>2.5623148088439001</v>
       </c>
       <c r="R8" s="5">
-        <v>2.2018163333432872</v>
+        <v>2.2031079405609999</v>
       </c>
       <c r="S8" s="5">
-        <v>1.5327815705376644</v>
+        <v>1.5344270847231001</v>
       </c>
       <c r="T8" s="5">
-        <v>1.5601066569108999</v>
+        <v>1.5619481804727</v>
       </c>
       <c r="U8" s="5">
-        <v>1.8334532807228714</v>
+        <v>1.8346402609329999</v>
       </c>
       <c r="V8">
-        <v>1.7325960383879628</v>
+        <v>1.7351684145971</v>
       </c>
       <c r="W8">
-        <v>1.7982644898455207</v>
+        <v>1.8090740709335</v>
       </c>
       <c r="X8">
-        <v>1.7198743659132214</v>
+        <v>1.73151891104</v>
       </c>
       <c r="Y8">
-        <v>1.6701919728214447</v>
+        <v>1.6723291907961</v>
       </c>
       <c r="Z8">
-        <v>1.4698719582185302</v>
+        <v>1.4795345846786001</v>
       </c>
       <c r="AA8">
-        <v>1.5450875895905685</v>
-      </c>
-    </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
+        <v>1.5431603341278</v>
+      </c>
+      <c r="AB8">
+        <v>1.5883411771974001</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" ht="15">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="B9" s="5">
-        <v>100</v>
+        <v>81.355893463524097</v>
       </c>
       <c r="C9" s="5">
-        <v>98.962436143911276</v>
+        <v>80.471719681401396</v>
       </c>
       <c r="D9" s="5">
-        <v>99.460165304227516</v>
+        <v>80.609311361243599</v>
       </c>
       <c r="E9" s="5">
-        <v>95.876543035235159</v>
+        <v>77.590223611182097</v>
       </c>
       <c r="F9" s="5">
-        <v>98.038048600271921</v>
+        <v>79.333096365451595</v>
       </c>
       <c r="G9" s="5">
-        <v>96.538157779095471</v>
+        <v>78.088717681487196</v>
       </c>
       <c r="H9" s="5">
-        <v>91.614467893196533</v>
+        <v>74.134480667471493</v>
       </c>
       <c r="I9" s="5">
-        <v>91.613385623621795</v>
+        <v>74.130731103572998</v>
       </c>
       <c r="J9" s="5">
-        <v>88.404346808584037</v>
+        <v>71.458429695375401</v>
       </c>
       <c r="K9" s="5">
-        <v>86.477115770642826</v>
+        <v>70.0155646975265</v>
       </c>
       <c r="L9" s="5">
-        <v>88.820573439873257</v>
+        <v>72.146214828201806</v>
       </c>
       <c r="M9" s="5">
-        <v>83.535858049541872</v>
+        <v>68.003247858797394</v>
       </c>
       <c r="N9" s="5">
-        <v>80.703994001765295</v>
+        <v>65.698801905038593</v>
       </c>
       <c r="O9" s="5">
-        <v>75.457475938170532</v>
+        <v>61.226316753597999</v>
       </c>
       <c r="P9" s="5">
-        <v>78.771243977857026</v>
+        <v>64.101570905482205</v>
       </c>
       <c r="Q9" s="5">
-        <v>70.1736873704142</v>
+        <v>57.035044959833698</v>
       </c>
       <c r="R9" s="5">
-        <v>70.573603089753064</v>
+        <v>57.3536902673182</v>
       </c>
       <c r="S9" s="5">
-        <v>67.911103481691399</v>
+        <v>55.369622438945697</v>
       </c>
       <c r="T9" s="5">
-        <v>63.52275336129577</v>
+        <v>51.632342495939</v>
       </c>
       <c r="U9" s="5">
-        <v>62.951621572276274</v>
+        <v>51.201981324866502</v>
       </c>
       <c r="V9">
-        <v>57.208303853632245</v>
+        <v>46.088401895287397</v>
       </c>
       <c r="W9">
-        <v>55.901982072960031</v>
+        <v>45.339204345936899</v>
       </c>
       <c r="X9">
-        <v>57.460533997405292</v>
+        <v>46.527344814210103</v>
       </c>
       <c r="Y9">
-        <v>56.530076161112198</v>
+        <v>45.830476296439898</v>
       </c>
       <c r="Z9">
-        <v>49.842299618889804</v>
+        <v>40.122335626709003</v>
       </c>
       <c r="AA9">
-        <v>50.9862576893971</v>
-      </c>
-    </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
-      <c r="A10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B10" s="5">
-        <v>81.926916902080919</v>
-      </c>
-      <c r="C10" s="5">
-        <v>81.076872823897091</v>
-      </c>
-      <c r="D10" s="5">
-        <v>80.609311361214196</v>
-      </c>
-      <c r="E10" s="5">
-        <v>77.590223611470222</v>
-      </c>
-      <c r="F10" s="5">
-        <v>79.333096365451155</v>
-      </c>
-      <c r="G10" s="5">
-        <v>78.088717681460011</v>
-      </c>
-      <c r="H10" s="5">
-        <v>74.134480667772266</v>
-      </c>
-      <c r="I10" s="5">
-        <v>74.130731103563448</v>
-      </c>
-      <c r="J10" s="5">
-        <v>71.458429696175685</v>
-      </c>
-      <c r="K10" s="5">
-        <v>70.015564693933513</v>
-      </c>
-      <c r="L10" s="5">
-        <v>72.146214824269393</v>
-      </c>
-      <c r="M10" s="5">
-        <v>68.003247859692294</v>
-      </c>
-      <c r="N10" s="5">
-        <v>65.698801905591779</v>
-      </c>
-      <c r="O10" s="5">
-        <v>61.226316753598717</v>
-      </c>
-      <c r="P10" s="5">
-        <v>64.101570906108108</v>
-      </c>
-      <c r="Q10" s="5">
-        <v>57.035044959775924</v>
-      </c>
-      <c r="R10" s="5">
-        <v>57.353690267643898</v>
-      </c>
-      <c r="S10" s="5">
-        <v>55.36962243913176</v>
-      </c>
-      <c r="T10" s="5">
-        <v>51.632342495905775</v>
-      </c>
-      <c r="U10" s="5">
-        <v>51.201981324786097</v>
-      </c>
-      <c r="V10">
-        <v>46.088401895283127</v>
-      </c>
-      <c r="W10">
-        <v>45.339204345986325</v>
-      </c>
-      <c r="X10">
-        <v>46.527344813795096</v>
-      </c>
-      <c r="Y10">
-        <v>45.83047629607767</v>
-      </c>
-      <c r="Z10">
-        <v>40.122335626762293</v>
-      </c>
-      <c r="AA10">
-        <v>40.634742310919513</v>
-      </c>
-      <c r="AB10">
-        <v>40.507483883738473</v>
+        <v>40.634742311027203</v>
+      </c>
+      <c r="AB9">
+        <v>40.605858416285798</v>
       </c>
     </row>
   </sheetData>
@@ -3626,28 +3555,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6465645E-7D70-4E1D-BBD4-D5D3D88FE1C3}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="88102e75-8a10-4cfc-9a6f-28ca16804fdc"/>
-    <ds:schemaRef ds:uri="a13e2855-205b-47c1-af91-45affc400dcd"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6465645E-7D70-4E1D-BBD4-D5D3D88FE1C3}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED60C750-2AA7-4A2B-AC93-5D702CFC5ECF}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{ED60C750-2AA7-4A2B-AC93-5D702CFC5ECF}"/>
 </file>
</xml_diff>